<commit_message>
add kotel and hvo new pages
</commit_message>
<xml_diff>
--- a/kaskad/production/sizod/zeh3linii/december/statistics12.24.xlsx
+++ b/kaskad/production/sizod/zeh3linii/december/statistics12.24.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DMITRY-SAIM\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Kaskad\Sambar\docs\kaskad\production\sizod\zeh3linii\december\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1101B276-A863-4F36-B307-B4F115EC7AA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="40">
   <si>
     <t>ДОТ ЭКО</t>
   </si>
@@ -135,22 +134,31 @@
     <t>перезапуск</t>
   </si>
   <si>
-    <t>нет данных</t>
-  </si>
-  <si>
     <t>перезапуск/герметичность</t>
   </si>
   <si>
     <t>замер угля/ нет воздуха</t>
   </si>
   <si>
-    <t>Ноябрь</t>
+    <t>не работали</t>
+  </si>
+  <si>
+    <t>Декабрь</t>
+  </si>
+  <si>
+    <t>замена сервопривода</t>
+  </si>
+  <si>
+    <t>настройка нуля</t>
+  </si>
+  <si>
+    <t>сервопривод настройка</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -635,7 +643,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -662,9 +670,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1298,11 +1303,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:S46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S42" sqref="S42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1329,13 +1334,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="71"/>
+      <c r="B2" s="69"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="70"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
@@ -1350,13 +1355,13 @@
       <c r="Q2" s="7"/>
     </row>
     <row r="3" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="102" t="s">
+      <c r="A3" s="101" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="102"/>
-      <c r="C3" s="102"/>
-      <c r="D3" s="102"/>
-      <c r="E3" s="102"/>
+      <c r="B3" s="101"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="101"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
@@ -1374,12 +1379,12 @@
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="98" t="s">
+      <c r="B4" s="97" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="99"/>
-      <c r="D4" s="99"/>
-      <c r="E4" s="100"/>
+      <c r="C4" s="98"/>
+      <c r="D4" s="98"/>
+      <c r="E4" s="99"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
@@ -1395,15 +1400,15 @@
       <c r="R4" s="5"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="95" t="s">
+      <c r="B5" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="96"/>
-      <c r="D5" s="96"/>
-      <c r="E5" s="97"/>
+      <c r="C5" s="95"/>
+      <c r="D5" s="95"/>
+      <c r="E5" s="96"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -1419,15 +1424,15 @@
       <c r="R5" s="3"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="92" t="s">
+      <c r="B6" s="91" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="93"/>
-      <c r="D6" s="93"/>
-      <c r="E6" s="94"/>
+      <c r="C6" s="92"/>
+      <c r="D6" s="92"/>
+      <c r="E6" s="93"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -1443,15 +1448,15 @@
       <c r="R6" s="3"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="89" t="s">
+      <c r="B7" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="90"/>
-      <c r="D7" s="90"/>
-      <c r="E7" s="91"/>
+      <c r="C7" s="89"/>
+      <c r="D7" s="89"/>
+      <c r="E7" s="90"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
@@ -1467,15 +1472,15 @@
       <c r="R7" s="3"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="86" t="s">
+      <c r="B8" s="85" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="87"/>
-      <c r="D8" s="87"/>
-      <c r="E8" s="88"/>
+      <c r="C8" s="86"/>
+      <c r="D8" s="86"/>
+      <c r="E8" s="87"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -1491,15 +1496,15 @@
       <c r="R8" s="3"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="83" t="s">
+      <c r="B9" s="82" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="84"/>
-      <c r="D9" s="84"/>
-      <c r="E9" s="85"/>
+      <c r="C9" s="83"/>
+      <c r="D9" s="83"/>
+      <c r="E9" s="84"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -1515,11 +1520,11 @@
       <c r="R9" s="3"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="35"/>
-      <c r="B10" s="101"/>
-      <c r="C10" s="101"/>
-      <c r="D10" s="101"/>
-      <c r="E10" s="101"/>
+      <c r="A10" s="34"/>
+      <c r="B10" s="100"/>
+      <c r="C10" s="100"/>
+      <c r="D10" s="100"/>
+      <c r="E10" s="100"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
@@ -1553,10 +1558,10 @@
       <c r="Q11" s="1"/>
     </row>
     <row r="12" spans="1:19" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="47" t="s">
+      <c r="A12" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="48">
+      <c r="B12" s="47">
         <v>2024</v>
       </c>
       <c r="C12" s="4"/>
@@ -1564,123 +1569,123 @@
       <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:19" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="78" t="s">
+      <c r="A13" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="103" t="s">
+      <c r="B13" s="102" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="104"/>
-      <c r="D13" s="104"/>
-      <c r="E13" s="104"/>
-      <c r="F13" s="104"/>
-      <c r="G13" s="104"/>
-      <c r="H13" s="104"/>
-      <c r="I13" s="104"/>
-      <c r="J13" s="104"/>
-      <c r="K13" s="104"/>
-      <c r="L13" s="104"/>
-      <c r="M13" s="104"/>
-      <c r="N13" s="104"/>
-      <c r="O13" s="104"/>
-      <c r="P13" s="104"/>
-      <c r="Q13" s="104"/>
-      <c r="R13" s="104"/>
-      <c r="S13" s="105"/>
+      <c r="C13" s="103"/>
+      <c r="D13" s="103"/>
+      <c r="E13" s="103"/>
+      <c r="F13" s="103"/>
+      <c r="G13" s="103"/>
+      <c r="H13" s="103"/>
+      <c r="I13" s="103"/>
+      <c r="J13" s="103"/>
+      <c r="K13" s="103"/>
+      <c r="L13" s="103"/>
+      <c r="M13" s="103"/>
+      <c r="N13" s="103"/>
+      <c r="O13" s="103"/>
+      <c r="P13" s="103"/>
+      <c r="Q13" s="103"/>
+      <c r="R13" s="103"/>
+      <c r="S13" s="104"/>
     </row>
     <row r="14" spans="1:19" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="79"/>
-      <c r="B14" s="74" t="s">
+      <c r="A14" s="78"/>
+      <c r="B14" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="74" t="s">
+      <c r="C14" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="107" t="s">
+      <c r="D14" s="106" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="74" t="s">
+      <c r="E14" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="113" t="s">
+      <c r="F14" s="112" t="s">
         <v>18</v>
       </c>
-      <c r="G14" s="114"/>
-      <c r="H14" s="76" t="s">
+      <c r="G14" s="113"/>
+      <c r="H14" s="75" t="s">
         <v>25</v>
       </c>
-      <c r="I14" s="77"/>
-      <c r="J14" s="81" t="s">
+      <c r="I14" s="76"/>
+      <c r="J14" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="K14" s="82"/>
-      <c r="L14" s="115" t="s">
+      <c r="K14" s="81"/>
+      <c r="L14" s="114" t="s">
         <v>21</v>
       </c>
-      <c r="M14" s="116"/>
-      <c r="N14" s="111" t="s">
+      <c r="M14" s="115"/>
+      <c r="N14" s="110" t="s">
         <v>20</v>
       </c>
-      <c r="O14" s="112"/>
-      <c r="P14" s="117" t="s">
+      <c r="O14" s="111"/>
+      <c r="P14" s="116" t="s">
         <v>9</v>
       </c>
-      <c r="Q14" s="118"/>
-      <c r="R14" s="109" t="s">
+      <c r="Q14" s="117"/>
+      <c r="R14" s="108" t="s">
         <v>22</v>
       </c>
-      <c r="S14" s="106" t="s">
+      <c r="S14" s="105" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="80"/>
-      <c r="B15" s="75"/>
-      <c r="C15" s="75"/>
-      <c r="D15" s="108"/>
-      <c r="E15" s="75"/>
-      <c r="F15" s="18" t="s">
+      <c r="A15" s="79"/>
+      <c r="B15" s="74"/>
+      <c r="C15" s="74"/>
+      <c r="D15" s="107"/>
+      <c r="E15" s="74"/>
+      <c r="F15" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="G15" s="19" t="s">
+      <c r="G15" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="H15" s="21" t="s">
+      <c r="H15" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="I15" s="22" t="s">
+      <c r="I15" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="J15" s="25" t="s">
+      <c r="J15" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="K15" s="26" t="s">
+      <c r="K15" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="L15" s="29" t="s">
+      <c r="L15" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="M15" s="30" t="s">
+      <c r="M15" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="N15" s="32" t="s">
+      <c r="N15" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="O15" s="33" t="s">
+      <c r="O15" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="P15" s="13" t="s">
+      <c r="P15" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="Q15" s="14" t="s">
+      <c r="Q15" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="R15" s="110"/>
-      <c r="S15" s="75"/>
+      <c r="R15" s="109"/>
+      <c r="S15" s="74"/>
     </row>
     <row r="16" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="46">
-        <v>45597</v>
+      <c r="A16" s="45">
+        <v>45627</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>7</v>
@@ -1694,34 +1699,34 @@
       <c r="E16" s="10">
         <v>0.25</v>
       </c>
-      <c r="F16" s="55" t="s">
-        <v>7</v>
-      </c>
-      <c r="G16" s="39" t="s">
-        <v>7</v>
-      </c>
-      <c r="H16" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="I16" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="J16" s="27">
+      <c r="F16" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="H16" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="I16" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="J16" s="26">
         <v>0.08</v>
       </c>
-      <c r="K16" s="28" t="s">
+      <c r="K16" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="L16" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="M16" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="N16" s="42" t="s">
-        <v>7</v>
-      </c>
-      <c r="O16" s="42" t="s">
+      <c r="L16" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="M16" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="N16" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="O16" s="41" t="s">
         <v>7</v>
       </c>
       <c r="P16" s="10" t="s">
@@ -1730,17 +1735,17 @@
       <c r="Q16" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="R16" s="36">
+      <c r="R16" s="35">
         <f>SUM(B16,C16,D16,E16,F16,H16,J16,L16,N16,P16)</f>
         <v>0.74999999999999989</v>
       </c>
-      <c r="S16" s="38" t="s">
+      <c r="S16" s="37" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="11">
-        <v>45598</v>
+        <v>45628</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>7</v>
@@ -1754,34 +1759,34 @@
       <c r="E17" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F17" s="55" t="s">
-        <v>7</v>
-      </c>
-      <c r="G17" s="39" t="s">
-        <v>7</v>
-      </c>
-      <c r="H17" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="I17" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="J17" s="27">
+      <c r="F17" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="G17" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="H17" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="I17" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="J17" s="26">
         <v>0.08</v>
       </c>
-      <c r="K17" s="28" t="s">
+      <c r="K17" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="L17" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="M17" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="N17" s="42" t="s">
-        <v>7</v>
-      </c>
-      <c r="O17" s="42" t="s">
+      <c r="L17" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="M17" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="N17" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="O17" s="41" t="s">
         <v>7</v>
       </c>
       <c r="P17" s="10" t="s">
@@ -1790,17 +1795,17 @@
       <c r="Q17" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="R17" s="37">
+      <c r="R17" s="36">
         <f t="shared" ref="R17:R32" si="0">SUM(B17,C17,D17,E17,F17,H17,J17,L17,N17,P17)</f>
         <v>0.08</v>
       </c>
-      <c r="S17" s="38" t="s">
+      <c r="S17" s="37" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="46">
-        <v>45599</v>
+      <c r="A18" s="45">
+        <v>45629</v>
       </c>
       <c r="B18" s="10" t="s">
         <v>7</v>
@@ -1814,34 +1819,34 @@
       <c r="E18" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="55" t="s">
-        <v>7</v>
-      </c>
-      <c r="G18" s="39" t="s">
-        <v>7</v>
-      </c>
-      <c r="H18" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="I18" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="J18" s="27">
+      <c r="F18" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="G18" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="H18" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="I18" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="J18" s="26">
         <v>0.17</v>
       </c>
-      <c r="K18" s="28" t="s">
+      <c r="K18" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="L18" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="M18" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="N18" s="42" t="s">
-        <v>7</v>
-      </c>
-      <c r="O18" s="42" t="s">
+      <c r="L18" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="M18" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="N18" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="O18" s="41" t="s">
         <v>7</v>
       </c>
       <c r="P18" s="10" t="s">
@@ -1850,47 +1855,77 @@
       <c r="Q18" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="R18" s="37">
+      <c r="R18" s="36">
         <f>SUM(B18,C18,D18,E18,F18,H18,J18,L18,N18,P18)</f>
         <v>0.17</v>
       </c>
-      <c r="S18" s="38" t="s">
+      <c r="S18" s="37" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="11">
-        <v>45600</v>
-      </c>
-      <c r="B19" s="60" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" s="61"/>
-      <c r="D19" s="61"/>
-      <c r="E19" s="61"/>
-      <c r="F19" s="61"/>
-      <c r="G19" s="61"/>
-      <c r="H19" s="61"/>
-      <c r="I19" s="61"/>
-      <c r="J19" s="61"/>
-      <c r="K19" s="61"/>
-      <c r="L19" s="61"/>
-      <c r="M19" s="61"/>
-      <c r="N19" s="61"/>
-      <c r="O19" s="61"/>
-      <c r="P19" s="61"/>
-      <c r="Q19" s="62"/>
-      <c r="R19" s="37">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="S19" s="38" t="s">
+        <v>45630</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="H19" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="I19" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="J19" s="26">
+        <v>0.17</v>
+      </c>
+      <c r="K19" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="L19" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="M19" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="N19" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="O19" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="P19" s="10">
+        <v>15</v>
+      </c>
+      <c r="Q19" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="R19" s="36">
+        <f>SUM(B19,C19,D19,E19,F19,H19,J19,L19,N19,P19)</f>
+        <v>15.17</v>
+      </c>
+      <c r="S19" s="37" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="46">
-        <v>45601</v>
+      <c r="A20" s="45">
+        <v>45631</v>
       </c>
       <c r="B20" s="10" t="s">
         <v>7</v>
@@ -1904,34 +1939,34 @@
       <c r="E20" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F20" s="55" t="s">
-        <v>7</v>
-      </c>
-      <c r="G20" s="39" t="s">
-        <v>7</v>
-      </c>
-      <c r="H20" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="I20" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="J20" s="27">
+      <c r="F20" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="G20" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="H20" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="I20" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="J20" s="26">
         <v>0.17</v>
       </c>
-      <c r="K20" s="28" t="s">
+      <c r="K20" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="L20" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="M20" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="N20" s="42" t="s">
-        <v>7</v>
-      </c>
-      <c r="O20" s="42" t="s">
+      <c r="L20" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="M20" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="N20" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="O20" s="41" t="s">
         <v>7</v>
       </c>
       <c r="P20" s="10" t="s">
@@ -1940,17 +1975,16 @@
       <c r="Q20" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="R20" s="37">
-        <f t="shared" si="0"/>
-        <v>0.17</v>
-      </c>
-      <c r="S20" s="38" t="s">
+      <c r="R20" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="S20" s="37" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="11">
-        <v>45602</v>
+        <v>45632</v>
       </c>
       <c r="B21" s="10" t="s">
         <v>7</v>
@@ -1964,53 +1998,53 @@
       <c r="E21" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F21" s="55" t="s">
-        <v>7</v>
-      </c>
-      <c r="G21" s="39" t="s">
-        <v>7</v>
-      </c>
-      <c r="H21" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="I21" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="J21" s="27">
+      <c r="F21" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="G21" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="H21" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="I21" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="J21" s="26">
         <v>0.17</v>
       </c>
-      <c r="K21" s="28" t="s">
+      <c r="K21" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="L21" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="M21" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="N21" s="42" t="s">
-        <v>7</v>
-      </c>
-      <c r="O21" s="42" t="s">
+      <c r="L21" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="M21" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="N21" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="O21" s="41" t="s">
         <v>7</v>
       </c>
       <c r="P21" s="10">
         <v>0.09</v>
       </c>
-      <c r="Q21" s="43" t="s">
+      <c r="Q21" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="R21" s="37">
+      <c r="R21" s="36">
         <f t="shared" si="0"/>
         <v>0.26</v>
       </c>
-      <c r="S21" s="38" t="s">
+      <c r="S21" s="37" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="46">
-        <v>45603</v>
+      <c r="A22" s="45">
+        <v>45633</v>
       </c>
       <c r="B22" s="10" t="s">
         <v>7</v>
@@ -2024,53 +2058,53 @@
       <c r="E22" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F22" s="55" t="s">
-        <v>7</v>
-      </c>
-      <c r="G22" s="39" t="s">
-        <v>7</v>
-      </c>
-      <c r="H22" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="I22" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="J22" s="27">
+      <c r="F22" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="H22" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="I22" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="J22" s="26">
         <v>0.17</v>
       </c>
-      <c r="K22" s="28" t="s">
+      <c r="K22" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="L22" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="M22" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="N22" s="42" t="s">
-        <v>7</v>
-      </c>
-      <c r="O22" s="42" t="s">
+      <c r="L22" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="M22" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="N22" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="O22" s="41" t="s">
         <v>7</v>
       </c>
       <c r="P22" s="10">
         <v>0.17</v>
       </c>
-      <c r="Q22" s="43" t="s">
+      <c r="Q22" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="R22" s="37">
+      <c r="R22" s="36">
         <f>SUM(B22,C22,D22,E22,F22,H22,J22,L22,N22,P22)</f>
         <v>0.51</v>
       </c>
-      <c r="S22" s="38" t="s">
+      <c r="S22" s="37" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="11">
-        <v>45604</v>
+        <v>45634</v>
       </c>
       <c r="B23" s="10" t="s">
         <v>7</v>
@@ -2084,53 +2118,53 @@
       <c r="E23" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F23" s="55" t="s">
-        <v>7</v>
-      </c>
-      <c r="G23" s="39" t="s">
-        <v>7</v>
-      </c>
-      <c r="H23" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="I23" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="J23" s="27">
+      <c r="F23" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="G23" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="H23" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="I23" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="J23" s="26">
         <v>0.17</v>
       </c>
-      <c r="K23" s="28" t="s">
+      <c r="K23" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="L23" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="M23" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="N23" s="42" t="s">
-        <v>7</v>
-      </c>
-      <c r="O23" s="42" t="s">
+      <c r="L23" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="M23" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="N23" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="O23" s="41" t="s">
         <v>7</v>
       </c>
       <c r="P23" s="10">
-        <v>0.09</v>
-      </c>
-      <c r="Q23" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="R23" s="37">
+        <v>2</v>
+      </c>
+      <c r="Q23" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="R23" s="36">
         <f t="shared" si="0"/>
-        <v>0.26</v>
-      </c>
-      <c r="S23" s="38" t="s">
+        <v>2.17</v>
+      </c>
+      <c r="S23" s="37" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="46">
-        <v>45605</v>
+      <c r="A24" s="45">
+        <v>45635</v>
       </c>
       <c r="B24" s="10" t="s">
         <v>7</v>
@@ -2144,53 +2178,53 @@
       <c r="E24" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F24" s="55" t="s">
-        <v>7</v>
-      </c>
-      <c r="G24" s="55" t="s">
-        <v>7</v>
-      </c>
-      <c r="H24" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="I24" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="J24" s="27">
+      <c r="F24" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="H24" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="I24" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="J24" s="26">
         <v>0.17</v>
       </c>
-      <c r="K24" s="28" t="s">
+      <c r="K24" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="L24" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="M24" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="N24" s="42" t="s">
-        <v>7</v>
-      </c>
-      <c r="O24" s="42" t="s">
-        <v>7</v>
-      </c>
-      <c r="P24" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q24" s="43" t="s">
-        <v>7</v>
-      </c>
-      <c r="R24" s="37">
+      <c r="L24" s="40">
+        <v>6</v>
+      </c>
+      <c r="M24" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="N24" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="O24" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="P24" s="10">
+        <v>6</v>
+      </c>
+      <c r="Q24" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="R24" s="36">
         <f t="shared" si="0"/>
-        <v>0.42000000000000004</v>
-      </c>
-      <c r="S24" s="38" t="s">
+        <v>12.42</v>
+      </c>
+      <c r="S24" s="37" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="11">
-        <v>45606</v>
+        <v>45636</v>
       </c>
       <c r="B25" s="10" t="s">
         <v>7</v>
@@ -2204,34 +2238,34 @@
       <c r="E25" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F25" s="55" t="s">
-        <v>7</v>
-      </c>
-      <c r="G25" s="55" t="s">
-        <v>7</v>
-      </c>
-      <c r="H25" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="I25" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="J25" s="27">
+      <c r="F25" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="G25" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="H25" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="I25" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="J25" s="26">
         <v>0.17</v>
       </c>
-      <c r="K25" s="28" t="s">
+      <c r="K25" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="L25" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="M25" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="N25" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="O25" s="42" t="s">
+      <c r="L25" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="M25" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="N25" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="O25" s="41" t="s">
         <v>7</v>
       </c>
       <c r="P25" s="10">
@@ -2240,17 +2274,17 @@
       <c r="Q25" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="R25" s="37">
+      <c r="R25" s="36">
         <f t="shared" si="0"/>
         <v>0.67</v>
       </c>
-      <c r="S25" s="38" t="s">
+      <c r="S25" s="37" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="46">
-        <v>45607</v>
+      <c r="A26" s="45">
+        <v>45638</v>
       </c>
       <c r="B26" s="10" t="s">
         <v>7</v>
@@ -2264,53 +2298,53 @@
       <c r="E26" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F26" s="55" t="s">
-        <v>7</v>
-      </c>
-      <c r="G26" s="55" t="s">
-        <v>7</v>
-      </c>
-      <c r="H26" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="I26" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="J26" s="27">
+      <c r="F26" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="G26" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="H26" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="I26" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="J26" s="26">
         <v>0.08</v>
       </c>
-      <c r="K26" s="27" t="s">
+      <c r="K26" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="L26" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="M26" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="N26" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="O26" s="42" t="s">
+      <c r="L26" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="M26" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="N26" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="O26" s="41" t="s">
         <v>7</v>
       </c>
       <c r="P26" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="Q26" s="43" t="s">
-        <v>7</v>
-      </c>
-      <c r="R26" s="37">
+      <c r="Q26" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="R26" s="36">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="S26" s="38" t="s">
+      <c r="S26" s="37" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="11">
-        <v>45608</v>
+        <v>45638</v>
       </c>
       <c r="B27" s="9" t="s">
         <v>7</v>
@@ -2324,34 +2358,34 @@
       <c r="E27" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F27" s="55" t="s">
-        <v>7</v>
-      </c>
-      <c r="G27" s="39" t="s">
-        <v>7</v>
-      </c>
-      <c r="H27" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="I27" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="J27" s="27">
+      <c r="F27" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="G27" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="H27" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="I27" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="J27" s="26">
         <v>0.17</v>
       </c>
-      <c r="K27" s="27" t="s">
+      <c r="K27" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="L27" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="M27" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="N27" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="O27" s="42" t="s">
+      <c r="L27" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="M27" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="N27" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="O27" s="41" t="s">
         <v>7</v>
       </c>
       <c r="P27" s="10">
@@ -2360,17 +2394,17 @@
       <c r="Q27" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="R27" s="37">
+      <c r="R27" s="36">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="S27" s="38" t="s">
+      <c r="S27" s="37" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="46">
-        <v>45609</v>
+      <c r="A28" s="45">
+        <v>45639</v>
       </c>
       <c r="B28" s="9" t="s">
         <v>7</v>
@@ -2384,34 +2418,34 @@
       <c r="E28" s="10">
         <v>0.25</v>
       </c>
-      <c r="F28" s="55" t="s">
-        <v>7</v>
-      </c>
-      <c r="G28" s="39" t="s">
-        <v>7</v>
-      </c>
-      <c r="H28" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="I28" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="J28" s="27">
+      <c r="F28" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="G28" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="H28" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="I28" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="J28" s="26">
         <v>0.17</v>
       </c>
-      <c r="K28" s="27" t="s">
+      <c r="K28" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="L28" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="M28" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="N28" s="42" t="s">
-        <v>7</v>
-      </c>
-      <c r="O28" s="42" t="s">
+      <c r="L28" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="M28" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="N28" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="O28" s="41" t="s">
         <v>7</v>
       </c>
       <c r="P28" s="10">
@@ -2420,17 +2454,17 @@
       <c r="Q28" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="R28" s="37">
+      <c r="R28" s="36">
         <f>SUM(B28,C28,D28,E28,F28,H28,J28,L28,N28,P28)</f>
         <v>1.19</v>
       </c>
-      <c r="S28" s="38" t="s">
+      <c r="S28" s="37" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="11">
-        <v>45610</v>
+        <v>45640</v>
       </c>
       <c r="B29" s="9" t="s">
         <v>7</v>
@@ -2444,53 +2478,53 @@
       <c r="E29" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F29" s="55" t="s">
-        <v>7</v>
-      </c>
-      <c r="G29" s="39" t="s">
-        <v>7</v>
-      </c>
-      <c r="H29" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="I29" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="J29" s="27">
+      <c r="F29" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="G29" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="H29" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="I29" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="J29" s="26">
         <v>0.5</v>
       </c>
-      <c r="K29" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="L29" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="M29" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="N29" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="O29" s="34" t="s">
+      <c r="K29" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="L29" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="M29" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="N29" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="O29" s="33" t="s">
         <v>7</v>
       </c>
       <c r="P29" s="10">
         <v>0.25</v>
       </c>
-      <c r="Q29" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="R29" s="37">
+      <c r="Q29" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="R29" s="36">
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
-      <c r="S29" s="38" t="s">
+      <c r="S29" s="37" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="46">
-        <v>45611</v>
+      <c r="A30" s="45">
+        <v>45641</v>
       </c>
       <c r="B30" s="9" t="s">
         <v>7</v>
@@ -2504,34 +2538,34 @@
       <c r="E30" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F30" s="55" t="s">
-        <v>7</v>
-      </c>
-      <c r="G30" s="39" t="s">
-        <v>7</v>
-      </c>
-      <c r="H30" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="I30" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="J30" s="27">
+      <c r="F30" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="G30" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="H30" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="I30" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="J30" s="26">
         <v>0.17</v>
       </c>
-      <c r="K30" s="56" t="s">
+      <c r="K30" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="L30" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="M30" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="N30" s="58" t="s">
-        <v>7</v>
-      </c>
-      <c r="O30" s="34" t="s">
+      <c r="L30" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="M30" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="N30" s="57" t="s">
+        <v>7</v>
+      </c>
+      <c r="O30" s="33" t="s">
         <v>7</v>
       </c>
       <c r="P30" s="10" t="s">
@@ -2540,17 +2574,17 @@
       <c r="Q30" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="R30" s="37">
+      <c r="R30" s="36">
         <f t="shared" si="0"/>
         <v>0.57999999999999996</v>
       </c>
-      <c r="S30" s="38" t="s">
+      <c r="S30" s="37" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="11">
-        <v>45612</v>
+        <v>45642</v>
       </c>
       <c r="B31" s="9" t="s">
         <v>7</v>
@@ -2564,34 +2598,34 @@
       <c r="E31" s="10">
         <v>0.25</v>
       </c>
-      <c r="F31" s="55" t="s">
-        <v>7</v>
-      </c>
-      <c r="G31" s="39" t="s">
-        <v>7</v>
-      </c>
-      <c r="H31" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="I31" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="J31" s="27">
+      <c r="F31" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="G31" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="H31" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="I31" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="J31" s="26">
         <v>0.08</v>
       </c>
-      <c r="K31" s="57" t="s">
+      <c r="K31" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="L31" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="M31" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="N31" s="59" t="s">
-        <v>7</v>
-      </c>
-      <c r="O31" s="42" t="s">
+      <c r="L31" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="M31" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="N31" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="O31" s="41" t="s">
         <v>7</v>
       </c>
       <c r="P31" s="10" t="s">
@@ -2600,17 +2634,17 @@
       <c r="Q31" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="R31" s="37">
+      <c r="R31" s="36">
         <f>SUM(B31,C31,D31,E31,F31,H31,J31,L31,N31,P31)</f>
         <v>0.33</v>
       </c>
-      <c r="S31" s="38" t="s">
+      <c r="S31" s="37" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="46">
-        <v>45613</v>
+      <c r="A32" s="45">
+        <v>45643</v>
       </c>
       <c r="B32" s="10" t="s">
         <v>7</v>
@@ -2624,53 +2658,53 @@
       <c r="E32" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F32" s="55" t="s">
-        <v>7</v>
-      </c>
-      <c r="G32" s="55" t="s">
-        <v>7</v>
-      </c>
-      <c r="H32" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="I32" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="J32" s="27">
+      <c r="F32" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="G32" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="H32" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="I32" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="J32" s="26">
         <v>0.25</v>
       </c>
-      <c r="K32" s="28" t="s">
+      <c r="K32" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="L32" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="M32" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="N32" s="42" t="s">
-        <v>7</v>
-      </c>
-      <c r="O32" s="42" t="s">
+      <c r="L32" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="M32" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="N32" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="O32" s="41" t="s">
         <v>7</v>
       </c>
       <c r="P32" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="Q32" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="R32" s="37">
+      <c r="Q32" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="R32" s="36">
         <f t="shared" si="0"/>
         <v>0.65999999999999992</v>
       </c>
-      <c r="S32" s="38" t="s">
+      <c r="S32" s="37" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="11">
-        <v>45614</v>
+        <v>45644</v>
       </c>
       <c r="B33" s="9" t="s">
         <v>7</v>
@@ -2684,53 +2718,53 @@
       <c r="E33" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F33" s="55" t="s">
-        <v>7</v>
-      </c>
-      <c r="G33" s="55" t="s">
-        <v>7</v>
-      </c>
-      <c r="H33" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="I33" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="J33" s="27">
+      <c r="F33" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="G33" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="H33" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="I33" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="J33" s="26">
         <v>0.17</v>
       </c>
-      <c r="K33" s="27" t="s">
+      <c r="K33" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="L33" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="M33" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="N33" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="O33" s="34" t="s">
+      <c r="L33" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="M33" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="N33" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="O33" s="33" t="s">
         <v>7</v>
       </c>
       <c r="P33" s="10">
         <v>0.17</v>
       </c>
-      <c r="Q33" s="43" t="s">
+      <c r="Q33" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="R33" s="37">
+      <c r="R33" s="36">
         <f t="shared" ref="R33:R44" si="1">SUM(B33,C33,D33,E33,F33,H33,J33,L33,N33,P33)</f>
         <v>0.34</v>
       </c>
-      <c r="S33" s="38" t="s">
+      <c r="S33" s="37" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="46">
-        <v>45615</v>
+      <c r="A34" s="45">
+        <v>45645</v>
       </c>
       <c r="B34" s="10" t="s">
         <v>7</v>
@@ -2744,53 +2778,53 @@
       <c r="E34" s="10">
         <v>0.5</v>
       </c>
-      <c r="F34" s="55" t="s">
-        <v>7</v>
-      </c>
-      <c r="G34" s="55" t="s">
-        <v>7</v>
-      </c>
-      <c r="H34" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="I34" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="J34" s="27">
+      <c r="F34" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="G34" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="H34" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="I34" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="J34" s="26">
         <v>0.08</v>
       </c>
-      <c r="K34" s="27" t="s">
+      <c r="K34" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="L34" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="M34" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="N34" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="O34" s="34" t="s">
+      <c r="L34" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="M34" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="N34" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="O34" s="33" t="s">
         <v>7</v>
       </c>
       <c r="P34" s="10">
         <v>0.25</v>
       </c>
-      <c r="Q34" s="43" t="s">
+      <c r="Q34" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="R34" s="37">
+      <c r="R34" s="36">
         <f t="shared" si="1"/>
         <v>1.08</v>
       </c>
-      <c r="S34" s="38" t="s">
+      <c r="S34" s="37" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="11">
-        <v>45616</v>
+        <v>45646</v>
       </c>
       <c r="B35" s="10" t="s">
         <v>7</v>
@@ -2804,34 +2838,34 @@
       <c r="E35" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F35" s="55" t="s">
-        <v>7</v>
-      </c>
-      <c r="G35" s="55" t="s">
-        <v>7</v>
-      </c>
-      <c r="H35" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="I35" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="J35" s="27">
+      <c r="F35" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="G35" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="H35" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="I35" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="J35" s="26">
         <v>0.17</v>
       </c>
-      <c r="K35" s="27" t="s">
+      <c r="K35" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="L35" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="M35" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="N35" s="42" t="s">
-        <v>7</v>
-      </c>
-      <c r="O35" s="34" t="s">
+      <c r="L35" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="M35" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="N35" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="O35" s="33" t="s">
         <v>7</v>
       </c>
       <c r="P35" s="10">
@@ -2840,17 +2874,17 @@
       <c r="Q35" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="R35" s="37">
+      <c r="R35" s="36">
         <f t="shared" si="1"/>
         <v>0.97000000000000008</v>
       </c>
-      <c r="S35" s="38" t="s">
+      <c r="S35" s="37" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="36" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="46">
-        <v>45617</v>
+      <c r="A36" s="45">
+        <v>45647</v>
       </c>
       <c r="B36" s="10" t="s">
         <v>7</v>
@@ -2864,34 +2898,34 @@
       <c r="E36" s="10">
         <v>0.17</v>
       </c>
-      <c r="F36" s="55" t="s">
-        <v>7</v>
-      </c>
-      <c r="G36" s="55" t="s">
-        <v>7</v>
-      </c>
-      <c r="H36" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="I36" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="J36" s="27">
+      <c r="F36" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="G36" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="H36" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="I36" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="J36" s="26">
         <v>0.17</v>
       </c>
-      <c r="K36" s="27" t="s">
+      <c r="K36" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="L36" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="M36" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="N36" s="42" t="s">
-        <v>7</v>
-      </c>
-      <c r="O36" s="42" t="s">
+      <c r="L36" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="M36" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="N36" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="O36" s="41" t="s">
         <v>7</v>
       </c>
       <c r="P36" s="10" t="s">
@@ -2900,17 +2934,17 @@
       <c r="Q36" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="R36" s="37">
+      <c r="R36" s="36">
         <f t="shared" si="1"/>
         <v>0.34</v>
       </c>
-      <c r="S36" s="38" t="s">
+      <c r="S36" s="37" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="37" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="11">
-        <v>45618</v>
+        <v>45648</v>
       </c>
       <c r="B37" s="10" t="s">
         <v>7</v>
@@ -2924,53 +2958,53 @@
       <c r="E37" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F37" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="G37" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="H37" s="49" t="s">
-        <v>7</v>
-      </c>
-      <c r="I37" s="49" t="s">
-        <v>7</v>
-      </c>
-      <c r="J37" s="27">
+      <c r="F37" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="G37" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="H37" s="48" t="s">
+        <v>7</v>
+      </c>
+      <c r="I37" s="48" t="s">
+        <v>7</v>
+      </c>
+      <c r="J37" s="26">
         <v>0.17</v>
       </c>
-      <c r="K37" s="28" t="s">
+      <c r="K37" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="L37" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="M37" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="N37" s="50" t="s">
-        <v>7</v>
-      </c>
-      <c r="O37" s="50" t="s">
+      <c r="L37" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="M37" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="N37" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="O37" s="49" t="s">
         <v>7</v>
       </c>
       <c r="P37" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="Q37" s="43" t="s">
+      <c r="Q37" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="R37" s="37">
+      <c r="R37" s="36">
         <f t="shared" si="1"/>
         <v>0.17</v>
       </c>
-      <c r="S37" s="38" t="s">
+      <c r="S37" s="37" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="38" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="46">
-        <v>45619</v>
+      <c r="A38" s="45">
+        <v>45649</v>
       </c>
       <c r="B38" s="9" t="s">
         <v>7</v>
@@ -2984,34 +3018,34 @@
       <c r="E38" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F38" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="G38" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="H38" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="I38" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="J38" s="27">
+      <c r="F38" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="G38" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="H38" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="I38" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="J38" s="26">
         <v>0.08</v>
       </c>
-      <c r="K38" s="27" t="s">
+      <c r="K38" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="L38" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="M38" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="N38" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="O38" s="34" t="s">
+      <c r="L38" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="M38" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="N38" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="O38" s="33" t="s">
         <v>7</v>
       </c>
       <c r="P38" s="10" t="s">
@@ -3020,17 +3054,17 @@
       <c r="Q38" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="R38" s="37">
+      <c r="R38" s="36">
         <f t="shared" si="1"/>
         <v>0.08</v>
       </c>
-      <c r="S38" s="38" t="s">
+      <c r="S38" s="37" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="39" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="11">
-        <v>45620</v>
+        <v>45650</v>
       </c>
       <c r="B39" s="9" t="s">
         <v>7</v>
@@ -3044,34 +3078,34 @@
       <c r="E39" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F39" s="44" t="s">
-        <v>7</v>
-      </c>
-      <c r="G39" s="39" t="s">
-        <v>7</v>
-      </c>
-      <c r="H39" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="I39" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="J39" s="27">
+      <c r="F39" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="G39" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="H39" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="I39" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="J39" s="26">
         <v>0.08</v>
       </c>
-      <c r="K39" s="27" t="s">
+      <c r="K39" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="L39" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="M39" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="N39" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="O39" s="34" t="s">
+      <c r="L39" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="M39" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="N39" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="O39" s="33" t="s">
         <v>7</v>
       </c>
       <c r="P39" s="10" t="s">
@@ -3080,17 +3114,17 @@
       <c r="Q39" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="R39" s="37">
+      <c r="R39" s="36">
         <f t="shared" si="1"/>
         <v>0.08</v>
       </c>
-      <c r="S39" s="38" t="s">
+      <c r="S39" s="37" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="40" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="46">
-        <v>45621</v>
+      <c r="A40" s="45">
+        <v>45651</v>
       </c>
       <c r="B40" s="9" t="s">
         <v>7</v>
@@ -3104,53 +3138,53 @@
       <c r="E40" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F40" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="G40" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="H40" s="49" t="s">
-        <v>7</v>
-      </c>
-      <c r="I40" s="49" t="s">
-        <v>7</v>
-      </c>
-      <c r="J40" s="27">
+      <c r="F40" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="G40" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="H40" s="48" t="s">
+        <v>7</v>
+      </c>
+      <c r="I40" s="48" t="s">
+        <v>7</v>
+      </c>
+      <c r="J40" s="26">
         <v>0.08</v>
       </c>
-      <c r="K40" s="27" t="s">
+      <c r="K40" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="L40" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="M40" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="N40" s="42" t="s">
-        <v>7</v>
-      </c>
-      <c r="O40" s="42" t="s">
+      <c r="L40" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="M40" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="N40" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="O40" s="41" t="s">
         <v>7</v>
       </c>
       <c r="P40" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="Q40" s="43" t="s">
+      <c r="Q40" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="R40" s="37">
+      <c r="R40" s="36">
         <f t="shared" si="1"/>
         <v>0.08</v>
       </c>
-      <c r="S40" s="38" t="s">
+      <c r="S40" s="37" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="41" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="11">
-        <v>45622</v>
+        <v>45652</v>
       </c>
       <c r="B41" s="9" t="s">
         <v>7</v>
@@ -3164,34 +3198,34 @@
       <c r="E41" s="10">
         <v>0.17</v>
       </c>
-      <c r="F41" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="G41" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="H41" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="I41" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="J41" s="27">
+      <c r="F41" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="G41" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="H41" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="I41" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="J41" s="26">
         <v>0.08</v>
       </c>
-      <c r="K41" s="27" t="s">
+      <c r="K41" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="L41" s="41">
+      <c r="L41" s="40">
         <v>0.17</v>
       </c>
-      <c r="M41" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="N41" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="O41" s="34" t="s">
+      <c r="M41" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="N41" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="O41" s="33" t="s">
         <v>7</v>
       </c>
       <c r="P41" s="10" t="s">
@@ -3200,312 +3234,192 @@
       <c r="Q41" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="R41" s="37">
+      <c r="R41" s="36">
         <f t="shared" si="1"/>
         <v>1.0900000000000001</v>
       </c>
-      <c r="S41" s="38" t="s">
+      <c r="S41" s="37" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="42" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="46">
-        <v>45623</v>
-      </c>
-      <c r="B42" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C42" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D42" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E42" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="F42" s="44" t="s">
-        <v>7</v>
-      </c>
-      <c r="G42" s="39" t="s">
-        <v>7</v>
-      </c>
-      <c r="H42" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="I42" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="J42" s="27">
-        <v>0.08</v>
-      </c>
-      <c r="K42" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="L42" s="41">
-        <v>0.25</v>
-      </c>
-      <c r="M42" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="N42" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="O42" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="P42" s="10">
-        <v>0.42</v>
-      </c>
-      <c r="Q42" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="R42" s="37">
+      <c r="A42" s="45">
+        <v>45653</v>
+      </c>
+      <c r="B42" s="59" t="s">
+        <v>35</v>
+      </c>
+      <c r="C42" s="60"/>
+      <c r="D42" s="60"/>
+      <c r="E42" s="60"/>
+      <c r="F42" s="60"/>
+      <c r="G42" s="60"/>
+      <c r="H42" s="60"/>
+      <c r="I42" s="60"/>
+      <c r="J42" s="60"/>
+      <c r="K42" s="60"/>
+      <c r="L42" s="60"/>
+      <c r="M42" s="60"/>
+      <c r="N42" s="60"/>
+      <c r="O42" s="60"/>
+      <c r="P42" s="60"/>
+      <c r="Q42" s="61"/>
+      <c r="R42" s="36">
         <f t="shared" si="1"/>
-        <v>0.75</v>
-      </c>
-      <c r="S42" s="38" t="s">
-        <v>29</v>
+        <v>0</v>
+      </c>
+      <c r="S42" s="37" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="43" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="11">
-        <v>45624</v>
-      </c>
-      <c r="B43" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C43" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D43" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E43" s="10">
-        <v>0.25</v>
-      </c>
-      <c r="F43" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="G43" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="H43" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="I43" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="J43" s="27">
-        <v>0.17</v>
-      </c>
-      <c r="K43" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="L43" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="M43" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="N43" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="O43" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="P43" s="10">
-        <v>0.08</v>
-      </c>
-      <c r="Q43" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="R43" s="37">
+        <v>45654</v>
+      </c>
+      <c r="B43" s="59" t="s">
+        <v>35</v>
+      </c>
+      <c r="C43" s="60"/>
+      <c r="D43" s="60"/>
+      <c r="E43" s="60"/>
+      <c r="F43" s="60"/>
+      <c r="G43" s="60"/>
+      <c r="H43" s="60"/>
+      <c r="I43" s="60"/>
+      <c r="J43" s="60"/>
+      <c r="K43" s="60"/>
+      <c r="L43" s="60"/>
+      <c r="M43" s="60"/>
+      <c r="N43" s="60"/>
+      <c r="O43" s="60"/>
+      <c r="P43" s="60"/>
+      <c r="Q43" s="61"/>
+      <c r="R43" s="36">
         <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-      <c r="S43" s="38" t="s">
-        <v>29</v>
+        <v>0</v>
+      </c>
+      <c r="S43" s="37" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="46">
-        <v>45625</v>
-      </c>
-      <c r="B44" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C44" s="10">
-        <v>0.25</v>
-      </c>
-      <c r="D44" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E44" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="F44" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="G44" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="H44" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="I44" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="J44" s="27">
-        <v>0.08</v>
-      </c>
-      <c r="K44" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="L44" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="M44" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="N44" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="O44" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="P44" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q44" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="R44" s="37">
+      <c r="A44" s="45">
+        <v>45655</v>
+      </c>
+      <c r="B44" s="59" t="s">
+        <v>35</v>
+      </c>
+      <c r="C44" s="60"/>
+      <c r="D44" s="60"/>
+      <c r="E44" s="60"/>
+      <c r="F44" s="60"/>
+      <c r="G44" s="60"/>
+      <c r="H44" s="60"/>
+      <c r="I44" s="60"/>
+      <c r="J44" s="60"/>
+      <c r="K44" s="60"/>
+      <c r="L44" s="60"/>
+      <c r="M44" s="60"/>
+      <c r="N44" s="60"/>
+      <c r="O44" s="60"/>
+      <c r="P44" s="60"/>
+      <c r="Q44" s="61"/>
+      <c r="R44" s="36">
         <f t="shared" si="1"/>
-        <v>0.33</v>
-      </c>
-      <c r="S44" s="38" t="s">
-        <v>29</v>
+        <v>0</v>
+      </c>
+      <c r="S44" s="37" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="45" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="11">
-        <v>45626</v>
-      </c>
-      <c r="B45" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C45" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D45" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E45" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="F45" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="G45" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="H45" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="I45" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="J45" s="27">
-        <v>0.17</v>
-      </c>
-      <c r="K45" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="L45" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="M45" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="N45" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="O45" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="P45" s="12">
-        <v>0.15</v>
-      </c>
-      <c r="Q45" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="R45" s="37">
+        <v>45656</v>
+      </c>
+      <c r="B45" s="59" t="s">
+        <v>35</v>
+      </c>
+      <c r="C45" s="60"/>
+      <c r="D45" s="60"/>
+      <c r="E45" s="60"/>
+      <c r="F45" s="60"/>
+      <c r="G45" s="60"/>
+      <c r="H45" s="60"/>
+      <c r="I45" s="60"/>
+      <c r="J45" s="60"/>
+      <c r="K45" s="60"/>
+      <c r="L45" s="60"/>
+      <c r="M45" s="60"/>
+      <c r="N45" s="60"/>
+      <c r="O45" s="60"/>
+      <c r="P45" s="60"/>
+      <c r="Q45" s="61"/>
+      <c r="R45" s="36">
         <f t="shared" ref="R45" si="2">SUM(B45,C45,D45,E45,F45,H45,J45,L45,N45,P45)</f>
-        <v>0.82000000000000006</v>
-      </c>
-      <c r="S45" s="38" t="s">
-        <v>29</v>
+        <v>0</v>
+      </c>
+      <c r="S45" s="37" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="46" spans="1:19" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="51" t="s">
+      <c r="A46" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="B46" s="53">
+      <c r="B46" s="52">
         <f>SUM(B16:B45)</f>
         <v>0</v>
       </c>
-      <c r="C46" s="52">
+      <c r="C46" s="51">
         <f>SUM(C16:C45)</f>
-        <v>2.5</v>
-      </c>
-      <c r="D46" s="54">
+        <v>2.25</v>
+      </c>
+      <c r="D46" s="53">
         <f>SUM(D16:D45)</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="E46" s="54">
+      <c r="E46" s="53">
         <f>SUM(E16:E45)</f>
-        <v>2.34</v>
-      </c>
-      <c r="F46" s="67">
+        <v>1.5899999999999999</v>
+      </c>
+      <c r="F46" s="66">
         <f>SUM(F16:F45)</f>
         <v>0</v>
       </c>
-      <c r="G46" s="68"/>
-      <c r="H46" s="67">
+      <c r="G46" s="67"/>
+      <c r="H46" s="66">
         <f>SUM(H16:H45)</f>
         <v>0</v>
       </c>
-      <c r="I46" s="68"/>
-      <c r="J46" s="63">
+      <c r="I46" s="67"/>
+      <c r="J46" s="62">
         <f>SUM(J16:J45)</f>
-        <v>4.3499999999999996</v>
-      </c>
-      <c r="K46" s="64"/>
-      <c r="L46" s="63">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="K46" s="63"/>
+      <c r="L46" s="62">
         <f>SUM(L16:L45)</f>
-        <v>0.42000000000000004</v>
-      </c>
-      <c r="M46" s="64"/>
-      <c r="N46" s="63">
+        <v>6.17</v>
+      </c>
+      <c r="M46" s="63"/>
+      <c r="N46" s="62">
         <f>SUM(N16:N45)</f>
         <v>0</v>
       </c>
-      <c r="O46" s="64"/>
-      <c r="P46" s="72">
+      <c r="O46" s="63"/>
+      <c r="P46" s="71">
         <f>SUM(P16:P45)</f>
-        <v>3.2199999999999998</v>
-      </c>
-      <c r="Q46" s="73"/>
-      <c r="R46" s="65">
+        <v>25.48</v>
+      </c>
+      <c r="Q46" s="72"/>
+      <c r="R46" s="64">
         <f>SUM(R16:R45)</f>
-        <v>13.930000000000001</v>
-      </c>
-      <c r="S46" s="66"/>
+        <v>40.44</v>
+      </c>
+      <c r="S46" s="65"/>
     </row>
   </sheetData>
-  <mergeCells count="31">
+  <mergeCells count="34">
     <mergeCell ref="B13:S13"/>
     <mergeCell ref="S14:S15"/>
     <mergeCell ref="D14:D15"/>
@@ -3530,13 +3444,16 @@
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B19:Q19"/>
     <mergeCell ref="N46:O46"/>
     <mergeCell ref="R46:S46"/>
     <mergeCell ref="F46:G46"/>
     <mergeCell ref="H46:I46"/>
     <mergeCell ref="J46:K46"/>
     <mergeCell ref="L46:M46"/>
+    <mergeCell ref="B42:Q42"/>
+    <mergeCell ref="B43:Q43"/>
+    <mergeCell ref="B44:Q44"/>
+    <mergeCell ref="B45:Q45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>